<commit_message>
update file phân công
</commit_message>
<xml_diff>
--- a/bản_phân_công_task.xlsx
+++ b/bản_phân_công_task.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PH Laptop\Desktop\workspace\Cybersoft\FE\react_movies_bc32e\ReactJSCapstone_MOVIES_BC32E_LongandKhang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PH Laptop\Desktop\workspace\Cybersoft\FE\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="8"/>
@@ -649,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="J5" s="14"/>
     </row>
@@ -685,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="8"/>
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J7" s="14"/>
     </row>

</xml_diff>